<commit_message>
Modificação do shape da população e teste de modificação de valor correspondente a aptidão
</commit_message>
<xml_diff>
--- a/Fluxo Rede/Logica T2 Trabalho IA.xlsx
+++ b/Fluxo Rede/Logica T2 Trabalho IA.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Desktop\T1_IA\Fluxo Rede\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8DC83D-B973-44FE-BABD-393A3E8F92DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CC9F0D-1506-440B-98E3-75BF3C2BB4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73366CEA-E3AA-4A22-9C04-767E2EC6BBF8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{73366CEA-E3AA-4A22-9C04-767E2EC6BBF8}"/>
   </bookViews>
   <sheets>
     <sheet name="Rede" sheetId="1" r:id="rId1"/>
+    <sheet name="Algoritmo Genético" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -22,6 +23,17 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Exemplo População</t>
+  </si>
+  <si>
+    <t>50x181</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63,9 +75,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -87,681 +102,36 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>316636</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>107961</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>365422</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>11486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>595469</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>7729</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="71" name="Fluxograma: Decisão 70">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{455B4373-D3BF-4E30-A07E-CD80F982371B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5193436" y="8642361"/>
-          <a:ext cx="2107633" cy="788768"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartDecision">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="pt-BR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200"/>
-            <a:t>Verifica Status Jogo</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
+      <xdr:colOff>366610</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>140033</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>351279</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>165971</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="72" name="Retângulo: Cantos Arredondados 71">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9384E04-B629-4A9E-80B9-D79ADF555E76}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4203700" y="10452433"/>
-          <a:ext cx="1024379" cy="559338"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="pt-BR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200"/>
-            <a:t>Rede joga</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>248664</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>117963</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>53843</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>143901</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="73" name="Retângulo: Cantos Arredondados 72">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BA4F7C2-E8E5-4B19-91BB-562CAEF96728}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5735064" y="10430363"/>
-          <a:ext cx="1024379" cy="559338"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="C00000"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="pt-BR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200"/>
-            <a:t>Encerra com boa nota</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>410589</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>140033</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>215768</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>165971</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="74" name="Retângulo: Cantos Arredondados 73">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4AEA1A-8A4D-4B46-B47D-0E30B5BA45B1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7116189" y="10452433"/>
-          <a:ext cx="1024379" cy="559338"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="C00000"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="pt-BR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1200"/>
-            <a:t>Encerra com nota ruim</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>448690</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>7729</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>151253</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>140033</xdr:rowOff>
+      <xdr:rowOff>121049</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="75" name="Conector reto 74">
+        <xdr:cNvPr id="76" name="Conector reto 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E61D7332-9049-4A17-9481-C397ED8086FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00ACFC35-8E2A-4314-A6C0-A9DBC5FFFFAC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:cxnSpLocks/>
           <a:stCxn id="71" idx="2"/>
-          <a:endCxn id="72" idx="0"/>
+          <a:endCxn id="73" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="4715890" y="9431129"/>
-          <a:ext cx="1531363" cy="1021304"/>
+          <a:off x="7044828" y="9476955"/>
+          <a:ext cx="1188" cy="1002532"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -791,636 +161,1166 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>151253</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>7729</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>151254</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>117963</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="76" name="Conector reto 75">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00ACFC35-8E2A-4314-A6C0-A9DBC5FFFFAC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-          <a:stCxn id="71" idx="2"/>
-          <a:endCxn id="73" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6247253" y="9431129"/>
-          <a:ext cx="1" cy="999234"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>151253</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>7729</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>313179</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>140033</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="77" name="Conector reto 76">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD94F700-F643-4709-B52B-89A6F39116A4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-          <a:stCxn id="71" idx="2"/>
-          <a:endCxn id="74" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6247253" y="9431129"/>
-          <a:ext cx="1381126" cy="1021304"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>358960</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>97874</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>84902</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>125802</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="78" name="CaixaDeTexto 36">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A6005CF-BCF9-49BD-9ADF-D8EDDAF544BC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4626160" y="9699074"/>
-          <a:ext cx="945142" cy="561328"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="pt-BR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1050"/>
-            <a:t>Ainda tem jogo</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="pt-BR" sz="1050"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>604771</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>29618</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>330713</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>78174</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="79" name="CaixaDeTexto 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A90526D9-8058-4DA0-8050-D71B78FC01A4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5481571" y="9808618"/>
-          <a:ext cx="945142" cy="404156"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="pt-BR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1050"/>
-            <a:t>Vitoria</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="pt-BR" sz="1050"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>179176</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>97874</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>514718</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>125802</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="80" name="CaixaDeTexto 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A34E6EB8-D21D-4EFD-B14D-FEF25560DB43}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6884776" y="9699074"/>
-          <a:ext cx="945142" cy="561328"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="pt-BR"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1050"/>
-            <a:t>Empate ou Derrota</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="pt-BR" sz="1050"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>149734</xdr:colOff>
+      <xdr:colOff>160814</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>151253</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>107961</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>422460</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>173591</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="81" name="Conector reto 80">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="39" name="Agrupar 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BABF068B-91B8-4B7A-94F0-8B893C8E9873}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F78ABD2-5A7A-6871-8C13-1C75253CFF05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:cxnSpLocks/>
-          <a:endCxn id="71" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6245734" y="7937500"/>
-          <a:ext cx="1519" cy="704861"/>
+          <a:off x="5061290" y="7897586"/>
+          <a:ext cx="3933670" cy="3062659"/>
+          <a:chOff x="4193223" y="7972425"/>
+          <a:chExt cx="3912579" cy="3091575"/>
         </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="71" name="Fluxograma: Decisão 70">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{455B4373-D3BF-4E30-A07E-CD80F982371B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5178196" y="8678556"/>
+            <a:ext cx="2092869" cy="796547"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartDecision">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Verifica Status Jogo</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="72" name="Retângulo: Cantos Arredondados 71">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9384E04-B629-4A9E-80B9-D79ADF555E76}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4193223" y="10494661"/>
+            <a:ext cx="1017711" cy="569339"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Rede joga</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="73" name="Retângulo: Cantos Arredondados 72">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BA4F7C2-E8E5-4B19-91BB-562CAEF96728}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5709823" y="10476401"/>
+            <a:ext cx="1027236" cy="559814"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Encerra com boa nota</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="74" name="Retângulo: Cantos Arredondados 73">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4AEA1A-8A4D-4B46-B47D-0E30B5BA45B1}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7088090" y="10494661"/>
+            <a:ext cx="1017712" cy="569339"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="C00000"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Encerra com nota ruim</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="75" name="Conector reto 74">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E61D7332-9049-4A17-9481-C397ED8086FC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:cxnSpLocks/>
+            <a:stCxn id="71" idx="2"/>
+            <a:endCxn id="72" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="4697316" y="9475103"/>
+            <a:ext cx="1526125" cy="1019558"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="77" name="Conector reto 76">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD94F700-F643-4709-B52B-89A6F39116A4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:cxnSpLocks/>
+            <a:stCxn id="71" idx="2"/>
+            <a:endCxn id="74" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6223441" y="9475103"/>
+            <a:ext cx="1378268" cy="1019558"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="78" name="CaixaDeTexto 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A6005CF-BCF9-49BD-9ADF-D8EDDAF544BC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4613301" y="9738127"/>
+            <a:ext cx="938475" cy="571329"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1050"/>
+              <a:t>Ainda tem jogo</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="pt-BR" sz="1050"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="79" name="CaixaDeTexto 37">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A90526D9-8058-4DA0-8050-D71B78FC01A4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5460616" y="9850369"/>
+            <a:ext cx="938475" cy="407649"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1050"/>
+              <a:t>Vitoria</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="pt-BR" sz="1050"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="80" name="CaixaDeTexto 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A34E6EB8-D21D-4EFD-B14D-FEF25560DB43}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6856677" y="9738127"/>
+            <a:ext cx="940856" cy="571329"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1050"/>
+              <a:t>Empate ou Derrota</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="pt-BR" sz="1050"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="81" name="Conector reto 80">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BABF068B-91B8-4B7A-94F0-8B893C8E9873}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:cxnSpLocks/>
+            <a:endCxn id="71" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6221922" y="7972425"/>
+            <a:ext cx="1519" cy="706131"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>96519</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>148087</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>174783</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>165971</xdr:rowOff>
+      <xdr:rowOff>173591</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -1435,8 +1335,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3136900" y="1435100"/>
-          <a:ext cx="8593587" cy="9576671"/>
+          <a:off x="3154316" y="1431653"/>
+          <a:ext cx="11100050" cy="9528592"/>
           <a:chOff x="3136900" y="1435100"/>
           <a:chExt cx="8593587" cy="9576671"/>
         </a:xfrm>
@@ -3942,7 +3842,7 @@
                   <a:pPr algn="ctr"/>
                   <a:r>
                     <a:rPr lang="pt-BR" sz="1200"/>
-                    <a:t>Fatia os pesos e os distribui na camada oculta e de saída</a:t>
+                    <a:t>Position chamada com a jogada atual</a:t>
                   </a:r>
                 </a:p>
               </xdr:txBody>
@@ -3961,7 +3861,7 @@
               <xdr:spPr>
                 <a:xfrm>
                   <a:off x="4470400" y="526722"/>
-                  <a:ext cx="1214886" cy="559795"/>
+                  <a:ext cx="1676163" cy="559795"/>
                 </a:xfrm>
                 <a:prstGeom prst="roundRect">
                   <a:avLst/>
@@ -4087,7 +3987,7 @@
                   <a:pPr algn="ctr"/>
                   <a:r>
                     <a:rPr lang="pt-BR" sz="1200"/>
-                    <a:t>Position chamada com a jogada atual</a:t>
+                    <a:t>Fatia os pesos e os distribui na camada oculta e de saída</a:t>
                   </a:r>
                 </a:p>
               </xdr:txBody>
@@ -4582,7 +4482,7 @@
               <xdr:spPr>
                 <a:xfrm>
                   <a:off x="3831083" y="791235"/>
-                  <a:ext cx="639317" cy="15385"/>
+                  <a:ext cx="639316" cy="15384"/>
                 </a:xfrm>
                 <a:prstGeom prst="line">
                   <a:avLst/>
@@ -4619,8 +4519,8 @@
               </xdr:nvCxnSpPr>
               <xdr:spPr>
                 <a:xfrm>
-                  <a:off x="5685286" y="806620"/>
-                  <a:ext cx="740914" cy="3360"/>
+                  <a:off x="6146563" y="806619"/>
+                  <a:ext cx="279637" cy="3360"/>
                 </a:xfrm>
                 <a:prstGeom prst="line">
                   <a:avLst/>
@@ -4811,19 +4711,19 @@
           </xdr:cNvPr>
           <xdr:cNvCxnSpPr>
             <a:stCxn id="72" idx="2"/>
-            <a:endCxn id="4" idx="0"/>
+            <a:endCxn id="3" idx="0"/>
           </xdr:cNvCxnSpPr>
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm rot="5400000" flipH="1" flipV="1">
-            <a:off x="1102141" y="5067570"/>
-            <a:ext cx="9557949" cy="2330453"/>
+            <a:off x="2312320" y="4150501"/>
+            <a:ext cx="9554589" cy="4167952"/>
           </a:xfrm>
           <a:prstGeom prst="bentConnector5">
             <a:avLst>
-              <a:gd name="adj1" fmla="val -2392"/>
-              <a:gd name="adj2" fmla="val -114987"/>
-              <a:gd name="adj3" fmla="val 102392"/>
+              <a:gd name="adj1" fmla="val -2382"/>
+              <a:gd name="adj2" fmla="val -61183"/>
+              <a:gd name="adj3" fmla="val 102382"/>
             </a:avLst>
           </a:prstGeom>
           <a:ln w="57150">
@@ -5152,8 +5052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E005F71-FAEC-4C33-8D91-D28EBE0DDA20}">
   <dimension ref="Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5165,4 +5065,31 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9CD0BE-2771-4FEA-957C-0D94BC110F5C}">
+  <dimension ref="B2:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finalização Fluxo Algoritmo Genético
</commit_message>
<xml_diff>
--- a/Fluxo Rede/Logica T2 Trabalho IA.xlsx
+++ b/Fluxo Rede/Logica T2 Trabalho IA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leona\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7f64a31289a2db41/Área de Trabalho/T1_IA/Fluxo Rede/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8DC83D-B973-44FE-BABD-393A3E8F92DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FF8DC83D-B973-44FE-BABD-393A3E8F92DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6F069F2-A8E8-442F-B22F-7DABED5E0321}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{73366CEA-E3AA-4A22-9C04-767E2EC6BBF8}"/>
   </bookViews>
@@ -4850,6 +4850,2202 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Conector reto 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E895FD03-0B47-4BBC-96C2-417548B516B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="32" idx="3"/>
+          <a:endCxn id="33" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="18097500" y="1854200"/>
+          <a:ext cx="736600" cy="38100"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="97" name="Agrupar 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9D0772F-172E-7E3C-18FF-0206031D5456}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="13271500" y="1384300"/>
+          <a:ext cx="12941300" cy="5918200"/>
+          <a:chOff x="13525500" y="1371600"/>
+          <a:chExt cx="12941300" cy="5918200"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="30" name="Retângulo: Cantos Arredondados 29">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D24EBDF1-40E0-BD23-C595-FA20C86B0F2B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="13525500" y="1397000"/>
+            <a:ext cx="2006600" cy="965200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Função</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> Heurística, recebe o status do jogos e qtd de jogadas feitas</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="Retângulo: Cantos Arredondados 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43935DF8-3BE8-4612-88D0-91687D6845D5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="16294100" y="1460500"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Atribui o valor</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> de retorno na no final do array de pesos</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="33" name="Retângulo: Cantos Arredondados 32">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E62880F-0A51-4E65-AA6E-4126ED180DF8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19088100" y="1422400"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Ao final do percorrimento</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> da população, é feito o Elitismo</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="35" name="Retângulo: Cantos Arredondados 34">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B280745-1278-49E8-8B17-8EB1BD81C372}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19177000" y="4000500"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Atribui o array</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> filtrado na posição zero da população_intermediária</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="36" name="Retângulo: Cantos Arredondados 35">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4F3E501-AA66-489A-8E08-7CF279D80952}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="21767800" y="1422400"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Até povoar</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> a população_intermediária, a </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Função</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> do Torneio é chamada</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="Retângulo: Cantos Arredondados 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D12A938-CE93-49ED-AB6B-27BF9DE6FFC8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19138900" y="2743200"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Procura</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> na última coluna da matriz da população o array com a maior nota</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="40" name="Retângulo: Cantos Arredondados 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{375DF38D-D3E9-47BE-821A-43886AB87DB8}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="21945600" y="2667000"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Busca</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> dois arrays aletaórios</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="42" name="Retângulo: Cantos Arredondados 41">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0360566-246B-4C02-8678-9917331911B6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="21945600" y="3937000"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Cria um novo array o</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> preenchendo com a média aritimética dos elementos dos arrays selecionados</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="43" name="Retângulo: Cantos Arredondados 42">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5467D331-8CE1-4EA9-ADD5-9A4226C2EBD3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="21983700" y="5194300"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Muda</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> o valor d</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>a</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> a</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t> última posição do array para 0 </a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="44" name="Retângulo: Cantos Arredondados 43">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8801C3D6-E767-45A1-8C8D-3A8B99993562}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="22072600" y="6451600"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200"/>
+              <a:t>Adicione</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t> esse array na população_intermediária</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="45" name="Retângulo: Cantos Arredondados 44">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D78E132-C9D4-479B-80CB-C6F0138D9881}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="24409400" y="1371600"/>
+            <a:ext cx="2057400" cy="838200"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="15000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle>
+            <a:defPPr>
+              <a:defRPr lang="pt-BR"/>
+            </a:defPPr>
+            <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl1pPr>
+            <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl2pPr>
+            <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl3pPr>
+            <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl4pPr>
+            <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl5pPr>
+            <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl6pPr>
+            <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl7pPr>
+            <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl8pPr>
+            <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+              <a:defRPr sz="1800" kern="1200">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:lvl9pPr>
+          </a:lstStyle>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="pt-BR" sz="1200" baseline="0"/>
+              <a:t>A população recebe a população_intermediária</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR" sz="1200"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="49" name="Conector reto 48">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CCC1701-D54F-8D23-4661-0F0D4EAB414A}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="30" idx="3"/>
+            <a:endCxn id="32" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="15532100" y="1879600"/>
+            <a:ext cx="762000" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="59" name="Conector reto 58">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8D78764-B882-49AC-9B25-C7587F7DC086}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="33" idx="2"/>
+            <a:endCxn id="37" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="20116800" y="2260600"/>
+            <a:ext cx="50800" cy="482600"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="63" name="Conector reto 62">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8765B9D2-913E-4C0A-B087-7BD097D3F00D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="37" idx="2"/>
+            <a:endCxn id="35" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="20167600" y="3581400"/>
+            <a:ext cx="38100" cy="419100"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="66" name="Conector reto 65">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F9ACD47-C7FF-48F4-A4EE-799CFED3A142}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="33" idx="3"/>
+            <a:endCxn id="36" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="21145500" y="1841500"/>
+            <a:ext cx="622300" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="69" name="Conector reto 68">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62701E1D-BB82-40BA-81A4-996B89F04CDC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="36" idx="3"/>
+            <a:endCxn id="45" idx="1"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="23825200" y="1790700"/>
+            <a:ext cx="584200" cy="50800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="84" name="Conector reto 83">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF1726B8-4284-41EA-B689-9F960FBD20A3}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="36" idx="2"/>
+            <a:endCxn id="40" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="22796500" y="2260600"/>
+            <a:ext cx="177800" cy="406400"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="88" name="Conector reto 87">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB071CCE-3E02-4B5A-B4B9-4DFC0EFBD1A2}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="40" idx="2"/>
+            <a:endCxn id="42" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="22974300" y="3505200"/>
+            <a:ext cx="0" cy="431800"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="91" name="Conector reto 90">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A431387-0BB3-4A05-AF3B-D2F2C2DE6FB6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="42" idx="2"/>
+            <a:endCxn id="43" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="22974300" y="4775200"/>
+            <a:ext cx="38100" cy="419100"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="94" name="Conector reto 93">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51427956-8EB4-4BBF-9217-5C565532921E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="43" idx="2"/>
+            <a:endCxn id="44" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="23012400" y="6032500"/>
+            <a:ext cx="88900" cy="419100"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="CaixaDeTexto 99">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDB8FC39-4E3C-4AA7-FB66-7D6CE3278C7F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="355600"/>
+          <a:ext cx="5486400" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="3200" b="1" kern="1200"/>
+            <a:t>Fluxo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="3200" b="1" kern="1200" baseline="0"/>
+            <a:t> Rede</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="3200" b="1" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="102" name="CaixaDeTexto 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CD5B461-AB4A-48D5-ADC9-1AF3927433C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16459200" y="533400"/>
+          <a:ext cx="5486400" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="3200" b="1" kern="1200"/>
+            <a:t>Fluxo</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="3200" b="1" kern="1200" baseline="0"/>
+            <a:t> Algortimo Genético</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="3200" b="1" kern="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5152,8 +7348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E005F71-FAEC-4C33-8D91-D28EBE0DDA20}">
   <dimension ref="Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>